<commit_message>
adição de gráficos e tabelas
</commit_message>
<xml_diff>
--- a/2019/tabelas_por_mes/tabelas_Final.xlsx
+++ b/2019/tabelas_por_mes/tabelas_Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vascoalbertofiliperibeiro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vascoalbertofiliperibeiro/R/SUS/2019/tabelas_por_mes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC19BE6F-9257-F248-9011-08A337DC06A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9598BC62-027D-2244-83BA-0541015D2479}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="14540" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="14540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="155">
   <si>
     <t>Mês</t>
   </si>
@@ -484,9 +484,6 @@
   </si>
   <si>
     <t>HOMENAGENS</t>
-  </si>
-  <si>
-    <t>ENCARGOS COM COLABORADRES</t>
   </si>
   <si>
     <t>BENGALEIRO</t>
@@ -523,6 +520,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1897,7 +1895,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1962,7 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2157,7 +2155,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2183,7 +2181,7 @@
         <v>147</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2235,7 +2233,7 @@
         <v>130</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2261,7 +2259,7 @@
         <v>130</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2287,7 +2285,7 @@
         <v>125</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2313,7 +2311,7 @@
         <v>137</v>
       </c>
       <c r="H13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2391,7 +2389,7 @@
         <v>127</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -2443,7 +2441,7 @@
         <v>137</v>
       </c>
       <c r="H18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -2469,7 +2467,7 @@
         <v>137</v>
       </c>
       <c r="H19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -6106,8 +6104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6118,7 +6116,7 @@
     <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6428,7 +6426,7 @@
         <v>3349.0999999999899</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="H12" t="s">
         <v>131</v>

</xml_diff>